<commit_message>
Testing on same task
</commit_message>
<xml_diff>
--- a/Results/Easy_task_validation.xlsx
+++ b/Results/Easy_task_validation.xlsx
@@ -424,13 +424,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Move Robot22 to location (6, 1) and remove the toolkit.
-</t>
+          <t>Move Robot32 to location (2, 9) and remove the toolkit.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>['Robot22']</t>
+          <t>['Robot32']</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -445,7 +444,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>(6, 1)</t>
+          <t>(2, 9)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -462,8 +461,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Move Robot6 to location (3, 8) and remove the liquid spill.
-</t>
+          <t>Move Robot6 to location (5, 4) and remove the liquid spill.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -483,7 +481,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>(3, 8)</t>
+          <t>(5, 4)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -500,18 +498,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Move Robot32 to location (12, 1) and remove the large debris.
-</t>
+          <t>Move Robot29 to location (5, 12) and remove the large debris.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['Robot32']</t>
+          <t>['Robot29']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['gripper']</t>
+          <t>['front loader']</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -521,7 +518,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>(12, 1)</t>
+          <t>(5, 12)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -538,13 +535,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Move Robot28 to location (9, 4) and remove the dust.
-</t>
+          <t>Move Robot48 to location (6, 6) and remove the dust.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['Robot28']</t>
+          <t>['Robot48']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -559,7 +555,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(9, 4)</t>
+          <t>(6, 6)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -576,8 +572,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Move Robot41 to location (7, 6) and remove the grass.
-</t>
+          <t>Move Robot41 to location (1, 8) and remove the grass.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -597,7 +592,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>(7, 6)</t>
+          <t>(1, 8)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -614,13 +609,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Move Robot50 to location (12, 12) and remove the small debris.
-</t>
+          <t>Move Robot10 to location (9, 5) and remove the small debris.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['Robot50']</t>
+          <t>['Robot10']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -635,7 +629,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>(12, 12)</t>
+          <t>(9, 5)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -652,13 +646,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Move Robot23 to location (9, 4) and remove the vehicle.
-</t>
+          <t>Move Robot13 to location (10, 10) and remove the vehicle.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['Robot23']</t>
+          <t>['Robot13']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -673,7 +666,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>(9, 4)</t>
+          <t>(10, 10)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -690,18 +683,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Move Robot42 to location (8, 8) and remove the construction materials.
-</t>
+          <t>Move Robot23 to location (8, 2) and remove the construction materials.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['Robot42']</t>
+          <t>['Robot23']</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['gripper']</t>
+          <t>['tow hook']</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -711,7 +703,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>(8, 8)</t>
+          <t>(8, 2)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -728,8 +720,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Move Robot24 to location (6, 10) and remove the tree branches.
-</t>
+          <t>Move Robot24 to location (11, 8) and remove the tree branches.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -749,7 +740,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>(6, 10)</t>
+          <t>(11, 8)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -766,8 +757,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Move Robot15 to location (9, 4) and remove the screws.
-</t>
+          <t>Move Robot15 to location (3, 8) and remove the screws.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -787,7 +777,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>(9, 4)</t>
+          <t>(3, 8)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">

</xml_diff>

<commit_message>
batch 6 made. added bad_prompt notebook for testing normal system
</commit_message>
<xml_diff>
--- a/Results/Easy_task_validation.xlsx
+++ b/Results/Easy_task_validation.xlsx
@@ -424,12 +424,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Move Robot32 to location (2, 9) and remove the toolkit.</t>
+          <t>Move Robot2 to location (2, 8) and remove the toolkit.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>['Robot32']</t>
+          <t>['Robot2']</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -444,7 +444,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>(2, 9)</t>
+          <t>(2, 8)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -461,12 +461,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Move Robot6 to location (5, 4) and remove the liquid spill.</t>
+          <t>Move Robot26 to location (11, 4) and remove the liquid spill.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['Robot6']</t>
+          <t>['Robot26']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>(5, 4)</t>
+          <t>(11, 4)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -498,17 +498,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Move Robot29 to location (5, 12) and remove the large debris.</t>
+          <t>Move Robot42 to location (9, 5) and remove the large debris.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['Robot29']</t>
+          <t>['Robot42']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['front loader']</t>
+          <t>['gripper']</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -518,7 +518,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>(5, 12)</t>
+          <t>(9, 5)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -535,7 +535,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Move Robot48 to location (6, 6) and remove the dust.</t>
+          <t>Move Robot48 to location (5, 6) and remove the dust.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -555,7 +555,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(6, 6)</t>
+          <t>(5, 6)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -572,12 +572,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Move Robot41 to location (1, 8) and remove the grass.</t>
+          <t>Move Robot31 to location (9, 4) and remove the grass.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['Robot41']</t>
+          <t>['Robot31']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -592,7 +592,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>(1, 8)</t>
+          <t>(9, 4)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -609,17 +609,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Move Robot10 to location (9, 5) and remove the small debris.</t>
+          <t>Move Robot8 to location (8, 12) and remove the small debris.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['Robot10']</t>
+          <t>['Robot8']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['vacuum']</t>
+          <t>['broom']</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>(9, 5)</t>
+          <t>(8, 12)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -646,12 +646,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Move Robot13 to location (10, 10) and remove the vehicle.</t>
+          <t>Move Robot23 to location (11, 1) and remove the vehicle.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['Robot13']</t>
+          <t>['Robot23']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -666,7 +666,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>(10, 10)</t>
+          <t>(11, 1)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -683,7 +683,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Move Robot23 to location (8, 2) and remove the construction materials.</t>
+          <t>Move Robot23 to location (12, 10) and remove the construction materials.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>(8, 2)</t>
+          <t>(12, 10)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -720,12 +720,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Move Robot24 to location (11, 8) and remove the tree branches.</t>
+          <t>Move Robot14 to location (7, 11) and remove the tree branches.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>['Robot24']</t>
+          <t>['Robot14']</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -740,7 +740,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>(11, 8)</t>
+          <t>(7, 11)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -757,7 +757,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Move Robot15 to location (3, 8) and remove the screws.</t>
+          <t>Move Robot15 to location (5, 3) and remove the screws.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -777,7 +777,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>(3, 8)</t>
+          <t>(5, 3)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">

</xml_diff>

<commit_message>
bad prompt test logged
</commit_message>
<xml_diff>
--- a/Results/Easy_task_validation.xlsx
+++ b/Results/Easy_task_validation.xlsx
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Move Robot2 to location (2, 8) and remove the toolkit.</t>
+          <t>Move Robot2 to location (11, 8) and remove the toolkit.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -444,7 +444,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>(2, 8)</t>
+          <t>(11, 8)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -461,7 +461,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Move Robot26 to location (11, 4) and remove the liquid spill.</t>
+          <t>Move Robot26 to location (4, 4) and remove the liquid spill.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>(11, 4)</t>
+          <t>(4, 4)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -498,7 +498,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Move Robot42 to location (9, 5) and remove the large debris.</t>
+          <t>Move Robot42 to location (9, 1) and remove the large debris.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -518,7 +518,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>(9, 5)</t>
+          <t>(9, 1)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -535,17 +535,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Move Robot48 to location (5, 6) and remove the dust.</t>
+          <t>Move Robot50 to location (7, 11) and remove the dust.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['Robot48']</t>
+          <t>['Robot50']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['broom']</t>
+          <t>['vacuum']</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -555,7 +555,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(5, 6)</t>
+          <t>(7, 11)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -572,12 +572,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Move Robot31 to location (9, 4) and remove the grass.</t>
+          <t>Move Robot41 to location (6, 12) and remove the grass.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['Robot31']</t>
+          <t>['Robot41']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -592,7 +592,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>(9, 4)</t>
+          <t>(6, 12)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -609,17 +609,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Move Robot8 to location (8, 12) and remove the small debris.</t>
+          <t>Move Robot50 to location (3, 1) and remove the small debris.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['Robot8']</t>
+          <t>['Robot50']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['broom']</t>
+          <t>['vacuum']</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>(8, 12)</t>
+          <t>(3, 1)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -646,12 +646,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Move Robot23 to location (11, 1) and remove the vehicle.</t>
+          <t>Move Robot13 to location (1, 4) and remove the vehicle.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['Robot23']</t>
+          <t>['Robot13']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -666,7 +666,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>(11, 1)</t>
+          <t>(1, 4)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -683,12 +683,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Move Robot23 to location (12, 10) and remove the construction materials.</t>
+          <t>Move Robot13 to location (11, 1) and remove the construction materials.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['Robot23']</t>
+          <t>['Robot13']</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>(12, 10)</t>
+          <t>(11, 1)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -720,7 +720,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Move Robot14 to location (7, 11) and remove the tree branches.</t>
+          <t>Move Robot14 to location (2, 10) and remove the tree branches.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -740,7 +740,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>(7, 11)</t>
+          <t>(2, 10)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -757,7 +757,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Move Robot15 to location (5, 3) and remove the screws.</t>
+          <t>Move Robot15 to location (8, 6) and remove the screws.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -777,7 +777,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>(5, 3)</t>
+          <t>(8, 6)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">

</xml_diff>